<commit_message>
Geração de imagem através do assistente
</commit_message>
<xml_diff>
--- a/gradeApp/static/assets/template_grade_CEAD.xlsx
+++ b/gradeApp/static/assets/template_grade_CEAD.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve">Nome do Curso</t>
   </si>
@@ -36,6 +36,9 @@
     <t>Carga-horária</t>
   </si>
   <si>
+    <t>Pré-requisito</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nome da disciplina</t>
   </si>
   <si>
@@ -43,6 +46,9 @@
   </si>
   <si>
     <t xml:space="preserve">Disciplina Convencional? Estágio? Etc...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(se houver)</t>
   </si>
 </sst>
 </file>
@@ -71,7 +77,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -86,12 +92,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.049989318521683403"/>
+        <bgColor theme="0" tint="-0.049989318521683403"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFAE1F25"/>
         <bgColor rgb="FFAE1F25"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -114,24 +126,83 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD0CECE"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFD0CECE"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFD0CECE"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="2" tint="-0.099978637043366805"/>
+      </left>
+      <right style="thin">
+        <color theme="2" tint="-0.099978637043366805"/>
+      </right>
+      <top style="thin">
+        <color theme="2" tint="-0.099978637043366805"/>
+      </top>
+      <bottom style="thin">
+        <color theme="2" tint="-0.099978637043366805"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD0CECE"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFD0CECE"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFD0CECE"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD0CECE"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFD0CECE"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="2" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="4" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="1" fillId="3" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="1" fillId="3" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="0" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="1" fillId="4" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="4" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="2" borderId="5" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf fontId="0" fillId="3" borderId="3" numFmtId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf fontId="2" fillId="2" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -650,75 +721,152 @@
     <col customWidth="1" min="2" max="2" style="1" width="51.28515625"/>
     <col customWidth="1" min="3" max="3" style="1" width="18.28515625"/>
     <col customWidth="1" min="4" max="4" style="1" width="46.5703125"/>
-    <col customWidth="1" min="5" max="5" style="1" width="18.42578125"/>
+    <col customWidth="1" min="5" max="5" style="2" width="18.42578125"/>
+    <col customWidth="1" min="6" max="6" style="3" width="24.140625"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="5"/>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="8" t="s">
         <v>6</v>
       </c>
+      <c r="F3" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="1">
+      <c r="A4" s="9">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="C4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1">
+      <c r="D4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="10">
         <v>60</v>
       </c>
+      <c r="F4" s="11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25">
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" ht="14.25">
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" ht="14.25">
+      <c r="F7" s="3"/>
     </row>
     <row r="8">
-      <c r="B8" s="7"/>
+      <c r="B8" s="12"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" ht="14.25">
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" ht="14.25">
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" ht="14.25">
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" ht="14.25">
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" ht="14.25">
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" ht="14.25">
+      <c r="F14" s="3"/>
     </row>
     <row r="15">
-      <c r="B15" s="7"/>
+      <c r="B15" s="12"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" ht="14.25">
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" ht="14.25">
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" ht="14.25">
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" ht="14.25">
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" ht="14.25">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" ht="14.25">
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" ht="14.25">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" ht="14.25">
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" ht="14.25">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" ht="14.25">
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" ht="14.25">
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" ht="14.25">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" ht="14.25">
+      <c r="F28" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>